<commit_message>
FEATURE: Get Last Update date CPI
</commit_message>
<xml_diff>
--- a/src/cpi/assets/report.xlsx
+++ b/src/cpi/assets/report.xlsx
@@ -49,10 +49,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Could not fetch the exchange Rates, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/indice-de-preco-no-consumidor/quadros/nacional</t>
-  </si>
-  <si>
-    <t>2022-09-06 23:36:08</t>
+    <t>Database failed to get xai-xai CPI</t>
+  </si>
+  <si>
+    <t>2022-09-07 22:25:55</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
IMPROVE: Data Format db
</commit_message>
<xml_diff>
--- a/src/cpi/assets/report.xlsx
+++ b/src/cpi/assets/report.xlsx
@@ -40,19 +40,19 @@
     <t>T1</t>
   </si>
   <si>
-    <t>CurrentCurrencyTrades</t>
-  </si>
-  <si>
-    <t>Update of current exchange rates</t>
+    <t>IPC</t>
+  </si>
+  <si>
+    <t>Monthly CPI</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Database failed to get niassa CPI</t>
-  </si>
-  <si>
-    <t>2022-09-08 01:31:08</t>
+    <t>Could not fetch the inhambane CPI, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/indice-de-preco-no-consumidor/quadros/inhambane</t>
+  </si>
+  <si>
+    <t>2022-09-08 19:44:11</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
FEATURE: Get CPI Loop
</commit_message>
<xml_diff>
--- a/src/cpi/assets/report.xlsx
+++ b/src/cpi/assets/report.xlsx
@@ -49,10 +49,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Could not fetch the inhambane CPI, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/indice-de-preco-no-consumidor/quadros/inhambane</t>
-  </si>
-  <si>
-    <t>2022-09-08 19:44:11</t>
+    <t>Database failed to get nacional CPI last update date</t>
+  </si>
+  <si>
+    <t>2022-09-08 22:13:46</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
FEATURE: Credit By Sector
</commit_message>
<xml_diff>
--- a/src/cpi/assets/report.xlsx
+++ b/src/cpi/assets/report.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Atualização dos indices de preços: Relatório da Ultima actividade</t>
   </si>
   <si>
-    <t>Task Code</t>
+    <t>Job Code</t>
   </si>
   <si>
     <t>Name</t>
@@ -37,7 +37,7 @@
     <t>date</t>
   </si>
   <si>
-    <t>T3</t>
+    <t>03-job-cpi</t>
   </si>
   <si>
     <t>IPC</t>
@@ -49,10 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Database failed to get nacional CPI last update date</t>
-  </si>
-  <si>
-    <t>2022-09-19 18:49:37</t>
+    <t>Was not possible to read None file</t>
   </si>
 </sst>
 </file>
@@ -494,8 +491,8 @@
       <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
+      <c r="G4">
+        <v>44855.73460388806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>